<commit_message>
guidelines of import excel
</commit_message>
<xml_diff>
--- a/assets/downloadables/DCF_Form_1.xlsx
+++ b/assets/downloadables/DCF_Form_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Data_Capture_Forms\DATA CAPTURE FORMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\dti_web_app_v2\assets\downloadables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
   </bookViews>
   <sheets>
     <sheet name="form1" sheetId="1" r:id="rId1"/>
@@ -957,40 +957,6 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1009,6 +975,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,7 +1231,7 @@
   </sheetPr>
   <dimension ref="A1:CA1002"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:BV5"/>
     </sheetView>
   </sheetViews>
@@ -1288,13 +1288,13 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
       <c r="O1" s="2"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="4"/>
@@ -1355,22 +1355,22 @@
       <c r="BT1" s="2"/>
     </row>
     <row r="2" spans="1:79" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="97"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7"/>
@@ -1390,11 +1390,11 @@
       <c r="AE2" s="10"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
-      <c r="AH2" s="91" t="s">
+      <c r="AH2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="AI2" s="92"/>
-      <c r="AJ2" s="93"/>
+      <c r="AI2" s="99"/>
+      <c r="AJ2" s="100"/>
       <c r="AK2" s="10"/>
       <c r="AL2" s="10"/>
       <c r="AM2" s="10"/>
@@ -1527,71 +1527,71 @@
       <c r="AE3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="94" t="s">
+      <c r="AF3" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="79"/>
-      <c r="AH3" s="80"/>
-      <c r="AI3" s="95" t="s">
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="102"/>
+      <c r="AI3" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="AJ3" s="79"/>
-      <c r="AK3" s="79"/>
-      <c r="AL3" s="79"/>
-      <c r="AM3" s="81"/>
-      <c r="AN3" s="83" t="s">
+      <c r="AJ3" s="91"/>
+      <c r="AK3" s="91"/>
+      <c r="AL3" s="91"/>
+      <c r="AM3" s="92"/>
+      <c r="AN3" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="AO3" s="84"/>
-      <c r="AP3" s="85"/>
-      <c r="AQ3" s="82" t="s">
+      <c r="AO3" s="88"/>
+      <c r="AP3" s="89"/>
+      <c r="AQ3" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="79"/>
-      <c r="AS3" s="79"/>
-      <c r="AT3" s="79"/>
-      <c r="AU3" s="79"/>
-      <c r="AV3" s="81"/>
-      <c r="AW3" s="82" t="s">
+      <c r="AR3" s="91"/>
+      <c r="AS3" s="91"/>
+      <c r="AT3" s="91"/>
+      <c r="AU3" s="91"/>
+      <c r="AV3" s="92"/>
+      <c r="AW3" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="AX3" s="79"/>
-      <c r="AY3" s="79"/>
-      <c r="AZ3" s="79"/>
-      <c r="BA3" s="79"/>
-      <c r="BB3" s="81"/>
+      <c r="AX3" s="91"/>
+      <c r="AY3" s="91"/>
+      <c r="AZ3" s="91"/>
+      <c r="BA3" s="91"/>
+      <c r="BB3" s="92"/>
       <c r="BC3" s="24" t="s">
         <v>69</v>
       </c>
       <c r="BD3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BE3" s="78" t="s">
+      <c r="BE3" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="BF3" s="79"/>
-      <c r="BG3" s="80"/>
-      <c r="BH3" s="78" t="s">
+      <c r="BF3" s="91"/>
+      <c r="BG3" s="102"/>
+      <c r="BH3" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="BI3" s="79"/>
-      <c r="BJ3" s="79"/>
-      <c r="BK3" s="79"/>
-      <c r="BL3" s="81"/>
-      <c r="BM3" s="78" t="s">
+      <c r="BI3" s="91"/>
+      <c r="BJ3" s="91"/>
+      <c r="BK3" s="91"/>
+      <c r="BL3" s="92"/>
+      <c r="BM3" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="BN3" s="79"/>
-      <c r="BO3" s="79"/>
-      <c r="BP3" s="79"/>
-      <c r="BQ3" s="81"/>
-      <c r="BR3" s="78" t="s">
+      <c r="BN3" s="91"/>
+      <c r="BO3" s="91"/>
+      <c r="BP3" s="91"/>
+      <c r="BQ3" s="92"/>
+      <c r="BR3" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="BS3" s="79"/>
-      <c r="BT3" s="79"/>
-      <c r="BU3" s="79"/>
-      <c r="BV3" s="81"/>
+      <c r="BS3" s="91"/>
+      <c r="BT3" s="91"/>
+      <c r="BU3" s="91"/>
+      <c r="BV3" s="92"/>
       <c r="BW3" s="25" t="s">
         <v>43</v>
       </c>
@@ -58675,6 +58675,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="BE3:BG3"/>
+    <mergeCell ref="BH3:BL3"/>
+    <mergeCell ref="BM3:BQ3"/>
+    <mergeCell ref="BR3:BV3"/>
+    <mergeCell ref="AW3:BB3"/>
     <mergeCell ref="AN3:AP3"/>
     <mergeCell ref="AQ3:AV3"/>
     <mergeCell ref="H1:N1"/>
@@ -58682,11 +58687,6 @@
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AF3:AH3"/>
     <mergeCell ref="AI3:AM3"/>
-    <mergeCell ref="BE3:BG3"/>
-    <mergeCell ref="BH3:BL3"/>
-    <mergeCell ref="BM3:BQ3"/>
-    <mergeCell ref="BR3:BV3"/>
-    <mergeCell ref="AW3:BB3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -58698,7 +58698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -58709,106 +58709,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="79" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="80" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="84" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="83" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="83" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="84" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="83" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="83" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="83" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="83" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="83" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="80" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="80" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
guidelines in template import excel
</commit_message>
<xml_diff>
--- a/assets/downloadables/DCF_Form_1.xlsx
+++ b/assets/downloadables/DCF_Form_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\dti_web_app_v2\assets\downloadables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\update template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t xml:space="preserve">DIP PREPARATION, REVIEW AND APPROVAL STATUS </t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>Refers to the total cost of Partner's FMI counterpart. Enter peso amount without comma.</t>
+  </si>
+  <si>
+    <t>RCUs</t>
+  </si>
+  <si>
+    <t>Input data using only number values. Avoid using any special characters or letters.</t>
+  </si>
+  <si>
+    <t>DIP details 14-73</t>
   </si>
 </sst>
 </file>
@@ -750,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -985,16 +994,21 @@
     <xf numFmtId="1" fontId="5" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1012,13 +1026,16 @@
     <xf numFmtId="4" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,7 +1257,7 @@
   </sheetPr>
   <dimension ref="A1:CA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1297,13 +1314,13 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
       <c r="O1" s="2"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="4"/>
@@ -1364,22 +1381,22 @@
       <c r="BT1" s="2"/>
     </row>
     <row r="2" spans="1:79" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="101"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7"/>
@@ -1399,11 +1416,11 @@
       <c r="AE2" s="10"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
-      <c r="AH2" s="99" t="s">
+      <c r="AH2" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="AI2" s="100"/>
-      <c r="AJ2" s="101"/>
+      <c r="AI2" s="103"/>
+      <c r="AJ2" s="104"/>
       <c r="AK2" s="10"/>
       <c r="AL2" s="10"/>
       <c r="AM2" s="10"/>
@@ -1536,71 +1553,71 @@
       <c r="AE3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="102" t="s">
+      <c r="AF3" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="103"/>
-      <c r="AI3" s="104" t="s">
+      <c r="AG3" s="90"/>
+      <c r="AH3" s="91"/>
+      <c r="AI3" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="AJ3" s="92"/>
-      <c r="AK3" s="92"/>
-      <c r="AL3" s="92"/>
-      <c r="AM3" s="93"/>
-      <c r="AN3" s="88" t="s">
+      <c r="AJ3" s="90"/>
+      <c r="AK3" s="90"/>
+      <c r="AL3" s="90"/>
+      <c r="AM3" s="92"/>
+      <c r="AN3" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="AO3" s="89"/>
-      <c r="AP3" s="90"/>
-      <c r="AQ3" s="91" t="s">
+      <c r="AO3" s="95"/>
+      <c r="AP3" s="96"/>
+      <c r="AQ3" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="92"/>
-      <c r="AS3" s="92"/>
-      <c r="AT3" s="92"/>
-      <c r="AU3" s="92"/>
-      <c r="AV3" s="93"/>
-      <c r="AW3" s="91" t="s">
+      <c r="AR3" s="90"/>
+      <c r="AS3" s="90"/>
+      <c r="AT3" s="90"/>
+      <c r="AU3" s="90"/>
+      <c r="AV3" s="92"/>
+      <c r="AW3" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="AX3" s="92"/>
-      <c r="AY3" s="92"/>
-      <c r="AZ3" s="92"/>
-      <c r="BA3" s="92"/>
-      <c r="BB3" s="93"/>
+      <c r="AX3" s="90"/>
+      <c r="AY3" s="90"/>
+      <c r="AZ3" s="90"/>
+      <c r="BA3" s="90"/>
+      <c r="BB3" s="92"/>
       <c r="BC3" s="24" t="s">
         <v>69</v>
       </c>
       <c r="BD3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BE3" s="105" t="s">
+      <c r="BE3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="BF3" s="92"/>
-      <c r="BG3" s="103"/>
-      <c r="BH3" s="105" t="s">
+      <c r="BF3" s="90"/>
+      <c r="BG3" s="91"/>
+      <c r="BH3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="BI3" s="92"/>
-      <c r="BJ3" s="92"/>
-      <c r="BK3" s="92"/>
-      <c r="BL3" s="93"/>
-      <c r="BM3" s="105" t="s">
+      <c r="BI3" s="90"/>
+      <c r="BJ3" s="90"/>
+      <c r="BK3" s="90"/>
+      <c r="BL3" s="92"/>
+      <c r="BM3" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="BN3" s="92"/>
-      <c r="BO3" s="92"/>
-      <c r="BP3" s="92"/>
-      <c r="BQ3" s="93"/>
-      <c r="BR3" s="105" t="s">
+      <c r="BN3" s="90"/>
+      <c r="BO3" s="90"/>
+      <c r="BP3" s="90"/>
+      <c r="BQ3" s="92"/>
+      <c r="BR3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="BS3" s="92"/>
-      <c r="BT3" s="92"/>
-      <c r="BU3" s="92"/>
-      <c r="BV3" s="93"/>
+      <c r="BS3" s="90"/>
+      <c r="BT3" s="90"/>
+      <c r="BU3" s="90"/>
+      <c r="BV3" s="92"/>
       <c r="BW3" s="25" t="s">
         <v>43</v>
       </c>
@@ -58684,11 +58701,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="BE3:BG3"/>
-    <mergeCell ref="BH3:BL3"/>
-    <mergeCell ref="BM3:BQ3"/>
-    <mergeCell ref="BR3:BV3"/>
-    <mergeCell ref="AW3:BB3"/>
     <mergeCell ref="AN3:AP3"/>
     <mergeCell ref="AQ3:AV3"/>
     <mergeCell ref="H1:N1"/>
@@ -58696,6 +58708,11 @@
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AF3:AH3"/>
     <mergeCell ref="AI3:AM3"/>
+    <mergeCell ref="BE3:BG3"/>
+    <mergeCell ref="BH3:BL3"/>
+    <mergeCell ref="BM3:BQ3"/>
+    <mergeCell ref="BR3:BV3"/>
+    <mergeCell ref="AW3:BB3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -58705,10 +58722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -58725,73 +58742,73 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+    <row r="2" spans="1:2" s="88" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="108" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B3" s="78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+    <row r="4" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B4" s="82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+    <row r="5" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="80" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
-        <v>78</v>
       </c>
       <c r="B5" s="81" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+    <row r="6" spans="1:2" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B7" s="82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
+    <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B8" s="81" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="81" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
-        <v>85</v>
+    <row r="9" spans="1:2" s="88" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="80" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="81" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B10" s="81" t="s">
         <v>84</v>
@@ -58799,30 +58816,50 @@
     </row>
     <row r="11" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B13" s="81" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79" t="s">
+    <row r="14" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B14" s="78" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79" t="s">
+    <row r="15" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B15" s="78" t="s">
         <v>89</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="109"/>
+      <c r="B16" s="109"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>